<commit_message>
Added sound and BSP finished
</commit_message>
<xml_diff>
--- a/DSA2 Final Grading Guide.xlsx
+++ b/DSA2 Final Grading Guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dynam\OneDrive\Documents\College\Semester 5\OpenGLFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D916701-AE3C-476E-B7AA-E8D4BA61464A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BF43E2-B330-4334-B0F8-5F26D4C94EAB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>Students</t>
   </si>
@@ -248,6 +248,27 @@
   </si>
   <si>
     <t>Two projects, cool stuff</t>
+  </si>
+  <si>
+    <t>Soundtrack is the medley of Galaga from Smash Brothers Ultimate (in Galaga)</t>
+  </si>
+  <si>
+    <t>A few audio effects from galaga included</t>
+  </si>
+  <si>
+    <t>shooting, enemy descent, and bullets killing enemies</t>
+  </si>
+  <si>
+    <t>All assets being used are automatically scaled to better fit the screen</t>
+  </si>
+  <si>
+    <t>The bullets are being sheared to be like the game (straight bullets)</t>
+  </si>
+  <si>
+    <t>Implemented broad phase collision detection using BSP tree (or at least what I imagine it to be for galaga)</t>
+  </si>
+  <si>
+    <t>Essentially, 3 lists of bools getting down to very specific numbers of where gameobjects are</t>
   </si>
 </sst>
 </file>
@@ -799,6 +820,84 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -827,84 +926,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1191,7 +1212,7 @@
   <dimension ref="A1:J143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1775,17 +1796,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="44" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1794,46 +1815,46 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="45" t="s">
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="47">
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="56">
         <f t="shared" ref="H2:H3" si="0">$F$59-$F$45+SUM($F$6:$F$21)</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="45" t="s">
+      <c r="A3" s="68"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="47">
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="56">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="65"/>
       <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1849,16 +1870,16 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1882,16 +1903,16 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
     </row>
     <row r="8" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
@@ -1926,16 +1947,16 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
     </row>
     <row r="11" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
@@ -1965,21 +1986,27 @@
       <c r="E12" s="9">
         <v>40</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
+      <c r="F12" s="9">
+        <v>40</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
     </row>
     <row r="14" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
@@ -2014,16 +2041,16 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="53"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
     </row>
     <row r="17" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
@@ -2035,8 +2062,12 @@
       <c r="E17" s="9">
         <v>5</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="10"/>
+      <c r="F17" s="9">
+        <v>5</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>77</v>
+      </c>
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2049,8 +2080,12 @@
       <c r="E18" s="9">
         <v>5</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="10"/>
+      <c r="F18" s="9">
+        <v>5</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2100,47 +2135,47 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:9" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="36"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="62"/>
       <c r="E22" s="11">
         <f>SUM(E2:E21)</f>
         <v>150</v>
       </c>
       <c r="F22" s="12">
         <f>SUM(F2:F21)</f>
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="20"/>
     </row>
     <row r="23" spans="1:9" ht="29.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="55" t="s">
+      <c r="A23" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="56"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="62" t="s">
+      <c r="A24" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="63"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
     </row>
     <row r="25" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
@@ -2167,16 +2202,16 @@
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="62" t="s">
+      <c r="A27" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="63"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="51"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
     </row>
     <row r="28" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
@@ -2239,16 +2274,16 @@
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="62" t="s">
+      <c r="A33" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="63"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="51"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
     </row>
     <row r="34" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
@@ -2323,16 +2358,16 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="62" t="s">
+      <c r="A40" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="63"/>
-      <c r="C40" s="63"/>
-      <c r="D40" s="64"/>
-      <c r="E40" s="51"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="51"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="48"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="48"/>
     </row>
     <row r="41" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
@@ -2385,12 +2420,12 @@
       <c r="J44" s="3"/>
     </row>
     <row r="45" spans="1:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="65" t="s">
+      <c r="A45" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="66"/>
-      <c r="C45" s="66"/>
-      <c r="D45" s="66"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
       <c r="E45" s="29">
         <f>SUM(E25:E44)</f>
         <v>0</v>
@@ -2403,16 +2438,16 @@
       <c r="H45" s="20"/>
     </row>
     <row r="46" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="52" t="s">
+      <c r="A46" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="53"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="58"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="52"/>
       <c r="I46" s="2"/>
     </row>
     <row r="47" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2425,9 +2460,15 @@
       <c r="E47" s="9">
         <v>5</v>
       </c>
-      <c r="F47" s="9"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
+      <c r="F47" s="9">
+        <v>5</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="48" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
@@ -2439,8 +2480,12 @@
       <c r="E48" s="9">
         <v>5</v>
       </c>
-      <c r="F48" s="9"/>
-      <c r="G48" s="10"/>
+      <c r="F48" s="9">
+        <v>5</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2582,37 +2627,37 @@
       <c r="H58" s="19"/>
     </row>
     <row r="59" spans="1:8" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="59" t="s">
+      <c r="A59" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="B59" s="60"/>
-      <c r="C59" s="60"/>
-      <c r="D59" s="61"/>
+      <c r="B59" s="41"/>
+      <c r="C59" s="41"/>
+      <c r="D59" s="42"/>
       <c r="E59" s="27">
         <f>SUM(E47:E58)</f>
         <v>175</v>
       </c>
       <c r="F59" s="26">
         <f>SUM(F47:F58)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
     </row>
     <row r="60" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="67" t="s">
+      <c r="A60" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B60" s="68"/>
-      <c r="C60" s="68"/>
-      <c r="D60" s="69"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="38"/>
+      <c r="D60" s="39"/>
       <c r="E60" s="25">
         <f>E59-E45+SUM(E6:E21)</f>
         <v>325</v>
       </c>
       <c r="F60" s="25">
         <f>$F$59-$F$45+SUM($F$6:$F$21)</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="G60" s="8"/>
       <c r="H60" s="8"/>
@@ -3192,35 +3237,35 @@
     <row r="143" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D15"/>
     <mergeCell ref="E23:H23"/>
     <mergeCell ref="A55:D55"/>
     <mergeCell ref="A56:D56"/>
@@ -3236,35 +3281,35 @@
     <mergeCell ref="E27:H27"/>
     <mergeCell ref="E33:H33"/>
     <mergeCell ref="E40:H40"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A35:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>